<commit_message>
Refactor - complete primate lentivirus extension
</commit_message>
<xml_diff>
--- a/tabular/extension/feline/feline-refseqs.xlsx
+++ b/tabular/extension/feline/feline-refseqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/retrovirus/Lentivirus-GLUE/tabular/extension/feline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5A7DC3-5755-7747-9E32-1584120B0333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1AAD3E-230F-024F-A982-C27B0D7208F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12380" yWindow="6400" windowWidth="27240" windowHeight="16440" xr2:uid="{A5ED6C89-0889-C641-A72D-22595E819967}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>